<commit_message>
making corrections after refactor
</commit_message>
<xml_diff>
--- a/EMT_Differences.xlsx
+++ b/EMT_Differences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Desktop\DCS_Job\python_experimentation\emt_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C6924BA-77DD-40A7-B21F-AA7C8042D5E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1B2FF6A-16CD-4532-BB9A-E153A5DEB436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="18000" windowHeight="9360" activeTab="4" xr2:uid="{8AE77D49-418D-49FB-9CF5-8ED033D4452D}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="18000" windowHeight="9360" activeTab="4" xr2:uid="{121EF5B2-5C8F-4F03-97BE-31C689F42806}"/>
   </bookViews>
   <sheets>
     <sheet name="Emitters" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="88">
   <si>
     <t>Base File: SPECTRE_OUTPUT_07032020.emt</t>
   </si>
@@ -144,9 +144,87 @@
     <t>MISSING</t>
   </si>
   <si>
+    <t>GENERATOR:</t>
+  </si>
+  <si>
+    <t>1'</t>
+  </si>
+  <si>
+    <t>$GENERATOR_KIND</t>
+  </si>
+  <si>
+    <t>type1'</t>
+  </si>
+  <si>
+    <t>$PCR</t>
+  </si>
+  <si>
+    <t>999N'</t>
+  </si>
+  <si>
+    <t>$SCAN_TYPE</t>
+  </si>
+  <si>
+    <t>J2'</t>
+  </si>
+  <si>
+    <t>J4'</t>
+  </si>
+  <si>
+    <t>$CSF</t>
+  </si>
+  <si>
+    <t>Px'</t>
+  </si>
+  <si>
+    <t>Pa'</t>
+  </si>
+  <si>
     <t>abc001xyz02'</t>
   </si>
   <si>
+    <t>FREQ_SEQUENCE:</t>
+  </si>
+  <si>
+    <t>$NUMBER_OF_SEGMENTS</t>
+  </si>
+  <si>
+    <t>$SEGMENT_TYPE</t>
+  </si>
+  <si>
+    <t>TYPE1'</t>
+  </si>
+  <si>
+    <t>PRI_SEGMENT:</t>
+  </si>
+  <si>
+    <t>$RF_BEAMS</t>
+  </si>
+  <si>
+    <t>5'</t>
+  </si>
+  <si>
+    <t>$RF_HOP_STEP</t>
+  </si>
+  <si>
+    <t>422'</t>
+  </si>
+  <si>
+    <t>$PRF</t>
+  </si>
+  <si>
+    <t>88'</t>
+  </si>
+  <si>
+    <t>$IPRF</t>
+  </si>
+  <si>
+    <t>678.00'</t>
+  </si>
+  <si>
+    <t>698.00'</t>
+  </si>
+  <si>
     <t>abc001xyz03'</t>
   </si>
   <si>
@@ -156,45 +234,42 @@
     <t>8'</t>
   </si>
   <si>
-    <t>GENERATOR:</t>
-  </si>
-  <si>
-    <t>1'</t>
-  </si>
-  <si>
-    <t>$GENERATOR_KIND</t>
-  </si>
-  <si>
-    <t>type1'</t>
-  </si>
-  <si>
-    <t>$PCR</t>
-  </si>
-  <si>
-    <t>999N'</t>
-  </si>
-  <si>
-    <t>$SCAN_TYPE</t>
-  </si>
-  <si>
-    <t>J4'</t>
-  </si>
-  <si>
     <t>J6'</t>
   </si>
   <si>
-    <t>$CSF</t>
-  </si>
-  <si>
-    <t>Pa'</t>
-  </si>
-  <si>
     <t>Paas'</t>
   </si>
   <si>
     <t>PRI_SEQUENCE:</t>
   </si>
   <si>
+    <t>$I_PRF</t>
+  </si>
+  <si>
+    <t>979.99'</t>
+  </si>
+  <si>
+    <t>$PD</t>
+  </si>
+  <si>
+    <t>999.99'</t>
+  </si>
+  <si>
+    <t>$COPD</t>
+  </si>
+  <si>
+    <t>999.99Z'</t>
+  </si>
+  <si>
+    <t>$SCAN_PERIOD</t>
+  </si>
+  <si>
+    <t>600.01'</t>
+  </si>
+  <si>
+    <t>$PRI</t>
+  </si>
+  <si>
     <t>3'</t>
   </si>
   <si>
@@ -211,6 +286,15 @@
   </si>
   <si>
     <t>TASCO'</t>
+  </si>
+  <si>
+    <t>abc003xyz'</t>
+  </si>
+  <si>
+    <t>abc005xyz'</t>
+  </si>
+  <si>
+    <t>abc006xyz'</t>
   </si>
   <si>
     <t>abc004xyz'</t>
@@ -592,8 +676,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664AF394-F592-480C-99E0-356379A432B8}">
-  <dimension ref="A1:Y9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8BDBC1-5FF7-4944-A7EB-B203C373D728}">
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -689,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -697,49 +781,91 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="M11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>59</v>
+      <c r="M12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -752,7 +878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E35922-76EE-4F4B-9A71-C78B17054D12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1AEF44-3866-4105-96CA-17773D9477DF}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -977,7 +1103,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>2</v>
@@ -989,7 +1115,7 @@
         <v>10</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -1126,7 +1252,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>2</v>
@@ -1138,7 +1264,7 @@
         <v>10</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -1160,7 +1286,7 @@
         <v>14</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>14</v>
@@ -1216,7 +1342,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="P29" s="2" t="s">
         <v>22</v>
@@ -1272,10 +1398,10 @@
         <v>34</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1288,8 +1414,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FFC6BE-B3B5-4FE2-B6C0-FDB2F547583A}">
-  <dimension ref="A1:Y8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F2F9C9-BAB1-4EA9-A29E-B73BA7C12450}">
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1352,13 +1478,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>2</v>
@@ -1370,91 +1496,373 @@
         <v>10</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="G7" s="5" t="s">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T7" s="6">
+      <c r="S17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="G8" s="5" t="s">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T8" s="6">
+      <c r="S18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T18" s="6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1467,12 +1875,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E588F83-A08A-4404-8C9D-6746B2F3745C}">
-  <dimension ref="A1:Y1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD478100-A137-41B9-B496-642E89CAD4DA}">
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1505,6 +1933,170 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="U6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="U7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="6"/>
+      <c r="U8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="U9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="U10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="U11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:L1"/>
@@ -1515,12 +2107,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A9E201-892D-4C43-BC1C-78B9F8221007}">
-  <dimension ref="A1:Y1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA70593-683C-4414-80C1-49F892E65B6F}">
+  <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1553,6 +2166,154 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:L1"/>

</xml_diff>